<commit_message>
1. Added final layout, config files. 2. Robot visualiser to visualise the robot movement. 3. Added delivery hub visualiser and integrated. 4. Code clean up ( removed unwanted files). 5. Bug fix in rpc interfaces in task manager. 6. Updated state machine to send package drop trigger (sitl) only once.
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="8">
   <si>
-    <t>(-,v,-,-)</t>
+    <t>(-,v,&gt;,-)</t>
   </si>
   <si>
     <t>(-,-,&gt;,&lt;)</t>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>(-,v,-,&lt;)</t>
+  </si>
+  <si>
+    <t>(-,v,-,-)</t>
   </si>
   <si>
     <t>(^,-,-,&lt;)</t>
@@ -381,550 +384,550 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -935,10 +938,10 @@
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -949,10 +952,10 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -963,10 +966,10 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -977,10 +980,10 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -991,10 +994,10 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1005,10 +1008,10 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -1019,10 +1022,10 @@
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -1033,10 +1036,10 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1047,10 +1050,10 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>

</xml_diff>